<commit_message>
Dodanie SprintBackologu, zrobienie szkicu projektu
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20340" windowHeight="7935"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20340" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
-    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
+    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,9 +16,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Product Backlog (lista wymagań)</t>
+  </si>
+  <si>
+    <t>Data Sprintu</t>
+  </si>
+  <si>
+    <t>Cel Sprintu</t>
+  </si>
+  <si>
+    <t>Zespół</t>
+  </si>
+  <si>
+    <t>Dąbrowska</t>
+  </si>
+  <si>
+    <t>Motyczko</t>
+  </si>
+  <si>
+    <t>Bogdał</t>
+  </si>
+  <si>
+    <t>Etgens</t>
+  </si>
+  <si>
+    <t>Bachorczyk</t>
+  </si>
+  <si>
+    <t>Zasoby [h]</t>
+  </si>
+  <si>
+    <t>Wykorzystane zasoby</t>
+  </si>
+  <si>
+    <t>Pozostałe zasoby</t>
+  </si>
+  <si>
+    <t>Nazwa</t>
+  </si>
+  <si>
+    <t>Kto wykonuje</t>
+  </si>
+  <si>
+    <t>Czas[h]</t>
+  </si>
+  <si>
+    <t>Code Review- kto</t>
+  </si>
+  <si>
+    <t>Code Review- uwagi</t>
+  </si>
+  <si>
+    <t>Stan Commitu</t>
+  </si>
+  <si>
+    <t>Story</t>
   </si>
 </sst>
 </file>
@@ -42,12 +96,54 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -62,9 +158,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -361,9 +485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -383,13 +505,182 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.25" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="14.25" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="18.375" customWidth="1"/>
+    <col min="6" max="6" width="17.625" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="52.5" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2"/>
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2"/>
+      <c r="B5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2"/>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2"/>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="8"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="8"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="8"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="8"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="8"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="8"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="8"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="8"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="8"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="8"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Uzupełnienie Backlogu produktu, Wersja I
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20340" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20340" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Product Backlog (lista wymagań)</t>
   </si>
@@ -73,13 +73,115 @@
   </si>
   <si>
     <t>Story</t>
+  </si>
+  <si>
+    <t>Kolejność</t>
+  </si>
+  <si>
+    <t>Oszacowanie czasu</t>
+  </si>
+  <si>
+    <t>Warość(priorytet)</t>
+  </si>
+  <si>
+    <t>Logistycy (sekretarki)</t>
+  </si>
+  <si>
+    <t>Mechanicy</t>
+  </si>
+  <si>
+    <t>Kierownik (ADMIN)</t>
+  </si>
+  <si>
+    <t>Księgowe</t>
+  </si>
+  <si>
+    <t>Dodawanie kont wszystkich pracowaników</t>
+  </si>
+  <si>
+    <t>Edycja kont, ustawianie haseł i loginów pracowników</t>
+  </si>
+  <si>
+    <t>Ustawia:imię, nazwisko, stanowisko, godziny pracy, urlopy, dostępność</t>
+  </si>
+  <si>
+    <t>Może podgladnac wszystkie operacje wykonywane przez kazdego pracownika</t>
+  </si>
+  <si>
+    <t>Widzi wszystkie opcje z kazdego konta</t>
+  </si>
+  <si>
+    <t>Po wejściu na stronę jest panel logowania i wyniki leleżne od stanowiska</t>
+  </si>
+  <si>
+    <t>Po zalogowaniu widzi 2 tryby</t>
+  </si>
+  <si>
+    <t>1. tryb- dane: imię, nazwisko, stanowisko, kalendarz z godzinami pracy, urlopami</t>
+  </si>
+  <si>
+    <t>2.tryb- zgłaszanie danej awarii :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyszukiwarka klientow po nazwisku i nr. rejestracyjnym pojazdu </t>
+  </si>
+  <si>
+    <t>Gdy jest klient, z jego konta ustala się nową wizytę, gdy nie jest, dodaje się go</t>
+  </si>
+  <si>
+    <t>Z konta klienta ustala nową wizytę (pole tekstowe)</t>
+  </si>
+  <si>
+    <t>Wybiera się z kalendarza dzień, w którym ma być wizyta</t>
+  </si>
+  <si>
+    <t>W wybranym dniu jest lista  mechaników (Zielony-wolny, Czerwony-Zajęty)</t>
+  </si>
+  <si>
+    <t>Wybiera się mechanika, ten automatycznie w bazie robi się Czerwony i akceptuje wizytę</t>
+  </si>
+  <si>
+    <t>Widzi charmonogram (kalendarz) dni kiedy ma wolne (czerwone) i kiedy ma być w pracy(zielone)</t>
+  </si>
+  <si>
+    <t>Zielony dzień jest klikalny, widzi tam rozpiskę godzinową oraz:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         *nieedytowalne pole z notatkami sekretarki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         *pola do uzupełnienia: cena swojej naprawy, cena za części, textbox- co zrobił</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         *Dwa przyciski: Zapisz i Nie udało się wykonać naprawy </t>
+  </si>
+  <si>
+    <t>Wszyscy</t>
+  </si>
+  <si>
+    <t>Dokładna wyszukiwarka usług, sortująca po:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Nazwisku, nr. rejestrecyjnym, po cenie usługi, za części i sumie, operatory: &lt; &gt;=</t>
+  </si>
+  <si>
+    <t>Jak wyszuka dane, pokazuje jej się opcja zaznaczenia tych znalezionych osób</t>
+  </si>
+  <si>
+    <t>Po zaznaczeniu uaktywnia się przyciski: Zapisz do pdf i zapisuje się na komputerze</t>
+  </si>
+  <si>
+    <t>Każdy ma zakładkę z wysuzkiwarką wykonanych usług i może szukać po:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   dacie (od -do), nr. rejestracyjnym, nazwisku klienta, nazwisku mechanika (Można łączyć)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,14 +191,20 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <color rgb="FF666666"/>
-      <name val="Verdana"/>
-      <family val="2"/>
+      <sz val="12"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="238"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +250,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9EE260"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF89"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -158,9 +296,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -189,12 +326,26 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF89"/>
+      <color rgb="FF9EE260"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -483,18 +634,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="41.25" customWidth="1"/>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="2" max="2" width="79.75" customWidth="1"/>
+    <col min="3" max="4" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15.75">
+      <c r="A1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -507,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -523,160 +833,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="52.5" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="2"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="2"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="2"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="2"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="2"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="2"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="8"/>
+      <c r="A11" s="7"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="8"/>
+      <c r="A12" s="7"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="8"/>
+      <c r="A13" s="7"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="8"/>
+      <c r="A14" s="7"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="8"/>
+      <c r="A15" s="7"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="8"/>
+      <c r="A16" s="7"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="8"/>
+      <c r="A17" s="7"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="8"/>
+      <c r="A18" s="7"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="8"/>
+      <c r="A19" s="7"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="8"/>
+      <c r="A20" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>